<commit_message>
Update Sales Entry Templates
</commit_message>
<xml_diff>
--- a/E2TGST/Resources/SalesEntriesA.xlsx
+++ b/E2TGST/Resources/SalesEntriesA.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Invoice Date</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>GSTIN/Party Ledger Name</t>
+  </si>
+  <si>
+    <t>Custom Sales Ledger Name</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -168,6 +171,10 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +490,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="SalesEntries"/>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,12 +505,13 @@
     <col min="5" max="5" width="9.140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="19" style="1" customWidth="1"/>
-    <col min="9" max="11" width="0" style="1" hidden="1"/>
-    <col min="12" max="16384" width="9.140625" style="1" hidden="1"/>
+    <col min="8" max="8" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -528,16 +536,35 @@
       <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -545,8 +572,9 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -554,6 +582,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" insertRows="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>

</xml_diff>